<commit_message>
av fusion avec qualification m16
Signed-off-by: zarma <daniel.dm@wanadoo.fr>
</commit_message>
<xml_diff>
--- a/crates/crates.xlsx
+++ b/crates/crates.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>crate</t>
   </si>
@@ -527,7 +527,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -720,6 +720,9 @@
       </c>
       <c r="C12" t="s">
         <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8">

</xml_diff>